<commit_message>
Harmonize parameters w Leander thesis
</commit_message>
<xml_diff>
--- a/Parameters/conversion_parameters.xlsx
+++ b/Parameters/conversion_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/mans3904_ox_ac_uk/Documents/DPhil/GEOH2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mans3904/Documents/GitHub/GEOH2-private/Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{CC005C10-9DF5-4F0E-B7F9-54620FD5BE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0408EBEE-1F10-49C8-BD10-E1FC35708512}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D70AFA-7E5E-B047-8AF2-268A0DA8727E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{18B0DDC9-B74C-4E09-B886-3EB1C823232B}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="14820" windowHeight="14480" activeTab="3" xr2:uid="{18B0DDC9-B74C-4E09-B886-3EB1C823232B}"/>
   </bookViews>
   <sheets>
     <sheet name="500 bar" sheetId="1" r:id="rId1"/>
@@ -460,19 +460,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA3769D-7505-4346-8C6B-6D06A7AD18B0}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -481,7 +483,7 @@
         <v>3.9444447600000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -489,7 +491,7 @@
         <v>298.14999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -497,7 +499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -505,7 +507,7 @@
         <v>1.4019999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -513,7 +515,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -521,7 +523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -529,12 +531,12 @@
         <v>40035</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>
@@ -546,20 +548,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B27EB1-F867-4EFB-A226-921B74E9D786}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -567,7 +571,7 @@
         <v>9.93</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -575,7 +579,7 @@
         <v>-2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -583,7 +587,7 @@
         <v>1781.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -592,15 +596,15 @@
         <v>300000000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -619,17 +623,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -637,7 +641,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -645,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -653,7 +657,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -661,7 +665,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -669,7 +673,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -677,7 +681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -694,19 +698,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE59E596-5506-44A6-B32A-5A1FC3D73A2D}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -714,7 +720,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -722,7 +728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -730,7 +736,7 @@
         <v>2.46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -738,7 +744,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -755,27 +761,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E224CE-91BF-435F-A756-EB96A1C22628}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
-        <v>3.109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2.8090000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -783,15 +791,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4">
-        <v>4.2537900000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0.75717000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -799,7 +807,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -816,35 +824,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBAAF98-B70E-424E-84FC-CE6118F32624}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -853,7 +863,7 @@
         <v>17262449.999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -861,7 +871,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Update to ReadMe to clarify spatial data prep and basic H2 plant params.
</commit_message>
<xml_diff>
--- a/Parameters/conversion_parameters.xlsx
+++ b/Parameters/conversion_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mans3904/Documents/GitHub/GEOH2-private/Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hert5576\PycharmProjects\GeoH2\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D70AFA-7E5E-B047-8AF2-268A0DA8727E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10189DE3-B4D1-479C-B57C-71D6C26A3513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="14820" windowHeight="14480" activeTab="3" xr2:uid="{18B0DDC9-B74C-4E09-B886-3EB1C823232B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{18B0DDC9-B74C-4E09-B886-3EB1C823232B}"/>
   </bookViews>
   <sheets>
     <sheet name="500 bar" sheetId="1" r:id="rId1"/>
@@ -460,30 +460,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA3769D-7505-4346-8C6B-6D06A7AD18B0}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <f>14200*((2.777778)*(0.000001))</f>
-        <v>3.9444447600000002E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.9399999999999999E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -491,7 +490,7 @@
         <v>298.14999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -499,7 +498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -507,7 +506,7 @@
         <v>1.4019999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -515,7 +514,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -523,7 +522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -531,7 +530,7 @@
         <v>40035</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -552,18 +551,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -571,7 +570,7 @@
         <v>9.93</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -579,7 +578,7 @@
         <v>-2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -587,7 +586,7 @@
         <v>1781.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -596,7 +595,7 @@
         <v>300000000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -604,7 +603,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -621,19 +620,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B15D9C4-0313-4761-ABC1-34D86A7C1894}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -641,15 +642,15 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -657,7 +658,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -665,7 +666,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -673,7 +674,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -681,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -698,21 +699,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE59E596-5506-44A6-B32A-5A1FC3D73A2D}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -720,7 +721,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -728,7 +729,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -736,7 +737,7 @@
         <v>2.46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -744,7 +745,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -765,17 +766,17 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -783,7 +784,7 @@
         <v>2.8090000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -791,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -799,7 +800,7 @@
         <v>0.75717000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -807,7 +808,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -828,17 +829,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -846,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -854,7 +855,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -863,7 +864,7 @@
         <v>17262449.999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -871,7 +872,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>

</xml_diff>